<commit_message>
Updated Test Cases for Supplier
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/03 TC - Suppliers.xlsx
+++ b/documentation/quality/Test Documents/03 TC - Suppliers.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HostedRBI\apc-softdev-it111-06\documentation\quality\Test Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-555" yWindow="2250" windowWidth="19440" windowHeight="8010"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1530,8 +1535,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1920,6 +1925,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1967,7 +1975,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1999,9 +2007,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2033,6 +2042,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2208,14 +2218,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="L3" sqref="L3:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -2225,7 +2235,7 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>151</v>
       </c>
@@ -2236,7 +2246,7 @@
       <c r="F1" s="54"/>
       <c r="G1" s="55"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
@@ -2262,7 +2272,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
@@ -2273,27 +2283,27 @@
       <c r="F3" s="51"/>
       <c r="G3" s="52"/>
       <c r="I3" s="56">
-        <f>AVERAGE(Sheet2!B17/88)</f>
+        <f>AVERAGE(Sheet2!B18/80)</f>
         <v>0</v>
       </c>
       <c r="J3" s="56">
-        <f>AVERAGE(Sheet2!C17/88)</f>
+        <f>AVERAGE(Sheet2!C18/80)</f>
         <v>0</v>
       </c>
       <c r="K3" s="56">
-        <f>AVERAGE(Sheet2!D17/88)</f>
-        <v>0.79545454545454541</v>
+        <f>AVERAGE(Sheet2!D18/80)</f>
+        <v>1</v>
       </c>
       <c r="L3" s="56">
-        <f>AVERAGE(Sheet2!E17/88)</f>
+        <f>AVERAGE(Sheet2!E18/80)</f>
         <v>0</v>
       </c>
       <c r="M3" s="56">
         <f>SUM(I3:L4)</f>
-        <v>0.79545454545454541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>150</v>
       </c>
@@ -2309,7 +2319,7 @@
       <c r="L4" s="56"/>
       <c r="M4" s="56"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -2322,7 +2332,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>2</v>
       </c>
@@ -2345,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="90.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:15" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
@@ -2362,7 +2372,7 @@
       </c>
       <c r="G7" s="36"/>
     </row>
-    <row r="8" spans="1:15" ht="150.75" customHeight="1" thickBot="1">
+    <row r="8" spans="1:15" ht="150.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
@@ -2388,7 +2398,7 @@
       <c r="N8" s="45"/>
       <c r="O8" s="46"/>
     </row>
-    <row r="9" spans="1:15" ht="135">
+    <row r="9" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
@@ -2405,7 +2415,7 @@
       </c>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:15" ht="210">
+    <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
@@ -2422,7 +2432,7 @@
       </c>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:15" ht="135">
+    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>20</v>
       </c>
@@ -2439,7 +2449,7 @@
       </c>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:15" s="11" customFormat="1">
+    <row r="12" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>4.0999999999999996</v>
       </c>
@@ -2452,7 +2462,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:15" ht="60">
+    <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>28</v>
       </c>
@@ -2469,7 +2479,7 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:15" ht="60">
+    <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>29</v>
       </c>
@@ -2486,7 +2496,7 @@
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>30</v>
       </c>
@@ -2503,7 +2513,7 @@
       </c>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:15" ht="30">
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>3.2</v>
       </c>
@@ -2516,7 +2526,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="1:7" ht="75">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>31</v>
       </c>
@@ -2533,7 +2543,7 @@
       </c>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" ht="150">
+    <row r="18" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>32</v>
       </c>
@@ -2550,7 +2560,7 @@
       </c>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" ht="135">
+    <row r="19" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>33</v>
       </c>
@@ -2567,7 +2577,7 @@
       </c>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" ht="135">
+    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>34</v>
       </c>
@@ -2584,7 +2594,7 @@
       </c>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" ht="60">
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>35</v>
       </c>
@@ -2601,7 +2611,7 @@
       </c>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="135">
+    <row r="22" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>36</v>
       </c>
@@ -2618,7 +2628,7 @@
       </c>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" ht="120">
+    <row r="23" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>37</v>
       </c>
@@ -2635,7 +2645,7 @@
       </c>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" ht="120">
+    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>38</v>
       </c>
@@ -2652,7 +2662,7 @@
       </c>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="120">
+    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>39</v>
       </c>
@@ -2669,7 +2679,7 @@
       </c>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" ht="165">
+    <row r="26" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>40</v>
       </c>
@@ -2686,7 +2696,7 @@
       </c>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7" ht="120">
+    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>41</v>
       </c>
@@ -2703,7 +2713,7 @@
       </c>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" ht="135">
+    <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>42</v>
       </c>
@@ -2720,7 +2730,7 @@
       </c>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:7" ht="150">
+    <row r="29" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>49</v>
       </c>
@@ -2737,7 +2747,7 @@
       </c>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>3.3</v>
       </c>
@@ -2750,7 +2760,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" ht="120">
+    <row r="31" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>54</v>
       </c>
@@ -2767,7 +2777,7 @@
       </c>
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="1:7" ht="135">
+    <row r="32" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>55</v>
       </c>
@@ -2784,7 +2794,7 @@
       </c>
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="1:7" ht="120">
+    <row r="33" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>56</v>
       </c>
@@ -2801,7 +2811,7 @@
       </c>
       <c r="G33" s="18"/>
     </row>
-    <row r="34" spans="1:7" ht="135">
+    <row r="34" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>57</v>
       </c>
@@ -2818,7 +2828,7 @@
       </c>
       <c r="G34" s="18"/>
     </row>
-    <row r="35" spans="1:7" ht="120">
+    <row r="35" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>58</v>
       </c>
@@ -2835,7 +2845,7 @@
       </c>
       <c r="G35" s="18"/>
     </row>
-    <row r="36" spans="1:7" ht="120">
+    <row r="36" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>59</v>
       </c>
@@ -2852,7 +2862,7 @@
       </c>
       <c r="G36" s="18"/>
     </row>
-    <row r="37" spans="1:7" ht="120">
+    <row r="37" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>60</v>
       </c>
@@ -2869,7 +2879,7 @@
       </c>
       <c r="G37" s="18"/>
     </row>
-    <row r="38" spans="1:7" ht="45">
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>61</v>
       </c>
@@ -2886,7 +2896,7 @@
       </c>
       <c r="G38" s="18"/>
     </row>
-    <row r="39" spans="1:7" ht="120">
+    <row r="39" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>62</v>
       </c>
@@ -2903,7 +2913,7 @@
       </c>
       <c r="G39" s="18"/>
     </row>
-    <row r="40" spans="1:7" ht="60">
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>63</v>
       </c>
@@ -2922,7 +2932,7 @@
       </c>
       <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="1:7" ht="45">
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>64</v>
       </c>
@@ -2941,7 +2951,7 @@
       </c>
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="1:7" ht="45">
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>251</v>
       </c>
@@ -2954,7 +2964,7 @@
       <c r="F42" s="8"/>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="1:7" ht="75">
+    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>198</v>
       </c>
@@ -2971,7 +2981,7 @@
       </c>
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="1:7" ht="75">
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>212</v>
       </c>
@@ -2988,7 +2998,7 @@
       </c>
       <c r="G44" s="18"/>
     </row>
-    <row r="45" spans="1:7" ht="75">
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>213</v>
       </c>
@@ -3005,7 +3015,7 @@
       </c>
       <c r="G45" s="18"/>
     </row>
-    <row r="46" spans="1:7" ht="75">
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>214</v>
       </c>
@@ -3022,7 +3032,7 @@
       </c>
       <c r="G46" s="18"/>
     </row>
-    <row r="47" spans="1:7" ht="60">
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>215</v>
       </c>
@@ -3039,7 +3049,7 @@
       </c>
       <c r="G47" s="18"/>
     </row>
-    <row r="48" spans="1:7" ht="60">
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>216</v>
       </c>
@@ -3056,7 +3066,7 @@
       </c>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:7" ht="60">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>217</v>
       </c>
@@ -3073,7 +3083,7 @@
       </c>
       <c r="G49" s="18"/>
     </row>
-    <row r="50" spans="1:7" ht="30">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>218</v>
       </c>
@@ -3090,7 +3100,7 @@
       </c>
       <c r="G50" s="18"/>
     </row>
-    <row r="51" spans="1:7" ht="45">
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>247</v>
       </c>
@@ -3107,7 +3117,7 @@
       </c>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:7" ht="30">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>3.4</v>
       </c>
@@ -3120,7 +3130,7 @@
       <c r="F52" s="9"/>
       <c r="G52" s="24"/>
     </row>
-    <row r="53" spans="1:7" ht="90">
+    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>76</v>
       </c>
@@ -3137,7 +3147,7 @@
       </c>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:7" ht="75">
+    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>77</v>
       </c>
@@ -3154,7 +3164,7 @@
       </c>
       <c r="G54" s="18"/>
     </row>
-    <row r="55" spans="1:7" ht="90">
+    <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>78</v>
       </c>
@@ -3171,7 +3181,7 @@
       </c>
       <c r="G55" s="18"/>
     </row>
-    <row r="56" spans="1:7" ht="75">
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>79</v>
       </c>
@@ -3188,7 +3198,7 @@
       </c>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:7" ht="75">
+    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>80</v>
       </c>
@@ -3205,7 +3215,7 @@
       </c>
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="1:7" ht="75">
+    <row r="58" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>81</v>
       </c>
@@ -3222,7 +3232,7 @@
       </c>
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="1:7" ht="150">
+    <row r="59" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>82</v>
       </c>
@@ -3239,7 +3249,7 @@
       </c>
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="1:7" ht="30">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
         <v>3.5</v>
       </c>
@@ -3252,7 +3262,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="24"/>
     </row>
-    <row r="61" spans="1:7" ht="75">
+    <row r="61" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>94</v>
       </c>
@@ -3269,7 +3279,7 @@
       </c>
       <c r="G61" s="18"/>
     </row>
-    <row r="62" spans="1:7" ht="60">
+    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>95</v>
       </c>
@@ -3286,7 +3296,7 @@
       </c>
       <c r="G62" s="18"/>
     </row>
-    <row r="63" spans="1:7" ht="75">
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>96</v>
       </c>
@@ -3303,7 +3313,7 @@
       </c>
       <c r="G63" s="18"/>
     </row>
-    <row r="64" spans="1:7" ht="150">
+    <row r="64" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>97</v>
       </c>
@@ -3320,7 +3330,7 @@
       </c>
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="1:7" ht="45">
+    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>98</v>
       </c>
@@ -3337,7 +3347,7 @@
       </c>
       <c r="G65" s="18"/>
     </row>
-    <row r="66" spans="1:7" ht="45">
+    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
         <v>252</v>
       </c>
@@ -3350,7 +3360,7 @@
       <c r="F66" s="15"/>
       <c r="G66" s="27"/>
     </row>
-    <row r="67" spans="1:7" ht="75">
+    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>107</v>
       </c>
@@ -3367,7 +3377,7 @@
       </c>
       <c r="G67" s="18"/>
     </row>
-    <row r="68" spans="1:7" ht="135">
+    <row r="68" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>109</v>
       </c>
@@ -3384,7 +3394,7 @@
       </c>
       <c r="G68" s="18"/>
     </row>
-    <row r="69" spans="1:7" ht="120">
+    <row r="69" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>110</v>
       </c>
@@ -3401,7 +3411,7 @@
       </c>
       <c r="G69" s="18"/>
     </row>
-    <row r="70" spans="1:7" ht="210">
+    <row r="70" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
         <v>111</v>
       </c>
@@ -3418,7 +3428,7 @@
       </c>
       <c r="G70" s="18"/>
     </row>
-    <row r="71" spans="1:7" ht="90">
+    <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>112</v>
       </c>
@@ -3435,7 +3445,7 @@
       </c>
       <c r="G71" s="18"/>
     </row>
-    <row r="72" spans="1:7" ht="165">
+    <row r="72" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>113</v>
       </c>
@@ -3452,7 +3462,7 @@
       </c>
       <c r="G72" s="18"/>
     </row>
-    <row r="73" spans="1:7" ht="45">
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>253</v>
       </c>
@@ -3465,7 +3475,7 @@
       <c r="F73" s="15"/>
       <c r="G73" s="27"/>
     </row>
-    <row r="74" spans="1:7" ht="60">
+    <row r="74" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>127</v>
       </c>
@@ -3482,7 +3492,7 @@
       </c>
       <c r="G74" s="18"/>
     </row>
-    <row r="75" spans="1:7" ht="150">
+    <row r="75" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>128</v>
       </c>
@@ -3499,7 +3509,7 @@
       </c>
       <c r="G75" s="18"/>
     </row>
-    <row r="76" spans="1:7" ht="60">
+    <row r="76" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>129</v>
       </c>
@@ -3516,7 +3526,7 @@
       </c>
       <c r="G76" s="18"/>
     </row>
-    <row r="77" spans="1:7" ht="45">
+    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
         <v>254</v>
       </c>
@@ -3529,7 +3539,7 @@
       <c r="F77" s="15"/>
       <c r="G77" s="27"/>
     </row>
-    <row r="78" spans="1:7" ht="60">
+    <row r="78" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>126</v>
       </c>
@@ -3546,7 +3556,7 @@
       </c>
       <c r="G78" s="18"/>
     </row>
-    <row r="79" spans="1:7" ht="165">
+    <row r="79" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>130</v>
       </c>
@@ -3563,7 +3573,7 @@
       </c>
       <c r="G79" s="18"/>
     </row>
-    <row r="80" spans="1:7" ht="165">
+    <row r="80" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>131</v>
       </c>
@@ -3580,7 +3590,7 @@
       </c>
       <c r="G80" s="18"/>
     </row>
-    <row r="81" spans="1:7" ht="75">
+    <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>132</v>
       </c>
@@ -3597,7 +3607,7 @@
       </c>
       <c r="G81" s="18"/>
     </row>
-    <row r="82" spans="1:7" ht="60">
+    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>133</v>
       </c>
@@ -3614,7 +3624,7 @@
       </c>
       <c r="G82" s="18"/>
     </row>
-    <row r="83" spans="1:7" ht="165">
+    <row r="83" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>134</v>
       </c>
@@ -3631,7 +3641,7 @@
       </c>
       <c r="G83" s="18"/>
     </row>
-    <row r="84" spans="1:7" ht="135">
+    <row r="84" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>135</v>
       </c>
@@ -3648,7 +3658,7 @@
       </c>
       <c r="G84" s="18"/>
     </row>
-    <row r="85" spans="1:7" ht="135">
+    <row r="85" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>136</v>
       </c>
@@ -3665,7 +3675,7 @@
       </c>
       <c r="G85" s="18"/>
     </row>
-    <row r="86" spans="1:7" ht="150">
+    <row r="86" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>137</v>
       </c>
@@ -3682,7 +3692,7 @@
       </c>
       <c r="G86" s="18"/>
     </row>
-    <row r="87" spans="1:7" ht="165">
+    <row r="87" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>138</v>
       </c>
@@ -3699,7 +3709,7 @@
       </c>
       <c r="G87" s="18"/>
     </row>
-    <row r="88" spans="1:7" ht="135">
+    <row r="88" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
         <v>139</v>
       </c>
@@ -3716,7 +3726,7 @@
       </c>
       <c r="G88" s="18"/>
     </row>
-    <row r="89" spans="1:7" ht="135">
+    <row r="89" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>140</v>
       </c>
@@ -3733,7 +3743,7 @@
       </c>
       <c r="G89" s="18"/>
     </row>
-    <row r="90" spans="1:7" ht="150">
+    <row r="90" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>141</v>
       </c>
@@ -3750,7 +3760,7 @@
       </c>
       <c r="G90" s="18"/>
     </row>
-    <row r="91" spans="1:7" ht="45">
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="33" t="s">
         <v>255</v>
       </c>
@@ -3763,7 +3773,7 @@
       <c r="F91" s="15"/>
       <c r="G91" s="27"/>
     </row>
-    <row r="92" spans="1:7" ht="195">
+    <row r="92" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>146</v>
       </c>
@@ -3780,7 +3790,7 @@
       </c>
       <c r="G92" s="18"/>
     </row>
-    <row r="93" spans="1:7" ht="90">
+    <row r="93" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>147</v>
       </c>
@@ -3797,7 +3807,7 @@
       </c>
       <c r="G93" s="18"/>
     </row>
-    <row r="94" spans="1:7" ht="210">
+    <row r="94" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>148</v>
       </c>
@@ -3814,7 +3824,7 @@
       </c>
       <c r="G94" s="18"/>
     </row>
-    <row r="95" spans="1:7" ht="30">
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>241</v>
       </c>
@@ -3831,7 +3841,7 @@
       </c>
       <c r="G95" s="18"/>
     </row>
-    <row r="96" spans="1:7" ht="60.75" thickBot="1">
+    <row r="96" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="28" t="s">
         <v>242</v>
       </c>
@@ -3848,22 +3858,22 @@
       </c>
       <c r="G96" s="32"/>
     </row>
-    <row r="312" spans="1:1">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:1">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="315" spans="1:1">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>8</v>
       </c>
@@ -3917,39 +3927,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -3966,12 +3976,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>4</v>
       </c>
       <c r="B7" s="43">
-        <f>COUNTIF(Sheet1!F8:F11, Sheet2!B6)</f>
+        <f>COUNTIF(Sheet1!F7:F11, Sheet2!B6)</f>
         <v>0</v>
       </c>
       <c r="C7" s="43">
@@ -3979,15 +3989,15 @@
         <v>0</v>
       </c>
       <c r="D7" s="43">
-        <f>COUNTIF(Sheet1!F8:F11, Sheet2!D6)</f>
-        <v>4</v>
+        <f>COUNTIF(Sheet1!F7:F11, Sheet2!D6)</f>
+        <v>5</v>
       </c>
       <c r="E7" s="43">
-        <f>COUNTIF(Sheet1!F8:F11, Sheet2!E6)</f>
+        <f>COUNTIF(Sheet1!F7:F11, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>4.0999999999999996</v>
       </c>
@@ -4008,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>4.2</v>
       </c>
@@ -4029,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>4.3</v>
       </c>
@@ -4050,150 +4060,169 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="42">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="42"/>
+      <c r="B11" s="43">
+        <f>COUNTIF(Sheet1!F43:F51, Sheet2!B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="43">
+        <f>COUNTIF(Sheet1!F43:F51, Sheet2!C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="43">
+        <f>COUNTIF(Sheet1!F43:F51, Sheet2!D6)</f>
+        <v>9</v>
+      </c>
+      <c r="E11" s="43">
+        <f>COUNTIF(Sheet1!F43:F51, Sheet2!E6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="42">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B12" s="43">
         <f>COUNTIF(Sheet1!F53:F59, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C12" s="43">
         <f>COUNTIF(Sheet1!F53:F59, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D12" s="43">
         <f>COUNTIF(Sheet1!F53:F59, Sheet2!D6)</f>
         <v>7</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E12" s="43">
         <f>COUNTIF(Sheet1!F53:F59, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="42">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="42">
         <v>4.5</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B13" s="43">
         <f>COUNTIF(Sheet1!F61:F65, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C13" s="43">
         <f>COUNTIF(Sheet1!F61:F65, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D13" s="43">
         <f>COUNTIF(Sheet1!F61:F65, Sheet2!D6)</f>
         <v>5</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E13" s="43">
         <f>COUNTIF(Sheet1!F61:F65, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="42" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B14" s="43">
         <f>COUNTIF(Sheet1!F67:F72, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C14" s="43">
         <f>COUNTIF(Sheet1!F67:F72, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D14" s="43">
         <f>COUNTIF(Sheet1!F67:F72, Sheet2!D6)</f>
         <v>6</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E14" s="43">
         <f>COUNTIF(Sheet1!F67:F72, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="42" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B15" s="43">
         <f>COUNTIF(Sheet1!F74:F76, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C15" s="43">
         <f>COUNTIF(Sheet1!F74:F76, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D15" s="43">
         <f>COUNTIF(Sheet1!F74:F76, Sheet2!D6)</f>
         <v>3</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E15" s="43">
         <f>COUNTIF(Sheet1!F74:F76, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="42" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B16" s="43">
         <f>COUNTIF(Sheet1!F78:F90, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C16" s="43">
         <f>COUNTIF(Sheet1!F78:F90, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D16" s="43">
         <f>COUNTIF(Sheet1!F78:F90, Sheet2!D6)</f>
         <v>13</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E16" s="43">
         <f>COUNTIF(Sheet1!F78:F90, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="42" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B17" s="43">
         <f>COUNTIF(Sheet1!F92:F96, Sheet2!B6)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C17" s="43">
         <f>COUNTIF(Sheet1!F92:F96, Sheet2!C6)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D17" s="43">
         <f>COUNTIF(Sheet1!F92:F96, Sheet2!D6)</f>
         <v>5</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E17" s="43">
         <f>COUNTIF(Sheet1!F92:F96, Sheet2!E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="42" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="B17">
-        <f>SUM(B7:B16)</f>
+      <c r="B18">
+        <f>SUM(B7:B17)</f>
         <v>0</v>
       </c>
-      <c r="C17">
-        <f>SUM(C7:C16)</f>
+      <c r="C18">
+        <f>SUM(C7:C17)</f>
         <v>0</v>
       </c>
-      <c r="D17">
-        <f>SUM(D7:D16)</f>
-        <v>70</v>
-      </c>
-      <c r="E17">
-        <f>SUM(E7:E16)</f>
+      <c r="D18">
+        <f>SUM(D7:D17)</f>
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <f>SUM(E7:E17)</f>
         <v>0</v>
       </c>
     </row>
@@ -4203,31 +4232,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>